<commit_message>
Algortimo de Prim practica_4
</commit_message>
<xml_diff>
--- a/lab/lab6/p4/tiempos.xlsx
+++ b/lab/lab6/p4/tiempos.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uo293697\Desktop\Algoritmia\lab\lab6\p4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/33b4c814603cc326/Escritorio/uo/2/Algoritmia/lab/lab6/p4/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_8051AD7E4EDCC674A8A22596081231382D13AB3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A199449C-F105-4592-ACFF-5186C004C70A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="8055"/>
+    <workbookView xWindow="-21710" yWindow="7020" windowWidth="21820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -35,7 +47,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -45,15 +60,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -61,12 +88,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -82,6 +129,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,83 +397,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D3:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="10.90625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+    <row r="3" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D4">
+    <row r="4" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="4">
         <v>256</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D5">
+      <c r="E4" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="4">
         <f>2*D4</f>
         <v>512</v>
       </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D6">
-        <f t="shared" ref="D6:D11" si="0">2*D5</f>
+      <c r="E5" s="5">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="4">
+        <f t="shared" ref="D6:D10" si="0">2*D5</f>
         <v>1024</v>
       </c>
-      <c r="E6">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D7">
+      <c r="E6" s="5">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-      <c r="E7">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D8">
+      <c r="E7" s="5">
+        <v>2.762</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="4">
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9">
+      <c r="E8" s="5">
+        <v>11.53</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>8192</v>
       </c>
-      <c r="E9">
-        <v>3.96</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>16384</v>
-      </c>
-      <c r="E10">
-        <v>12.85</v>
+      <c r="E9" s="5">
+        <v>53.460999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="4">
+        <v>10000</v>
+      </c>
+      <c r="E10" s="5">
+        <v>78.015000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>